<commit_message>
Verificacion de existencia del codigo dentro del Excel
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>No</t>
   </si>
@@ -96,6 +96,30 @@
   </si>
   <si>
     <t>Jez Humble</t>
+  </si>
+  <si>
+    <t>El que se duerme pierde</t>
+  </si>
+  <si>
+    <t>Tom Peter</t>
+  </si>
+  <si>
+    <t>Sin lugar a duda</t>
+  </si>
+  <si>
+    <t>Ana Gutierrez</t>
+  </si>
+  <si>
+    <t>El arte de dormir</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Buscando a Nemo</t>
+  </si>
+  <si>
+    <t>Humble Po</t>
   </si>
 </sst>
 </file>
@@ -422,8 +446,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -580,6 +604,118 @@
         <v>41.0</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizacion del nombre de autor y el precio segun el numero de identificacion mas la validacion de ingreso de los campos, sea numerico o de tipo string para evitar que el programa se crashee.
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>No</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Humble Po</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Petrosky</t>
   </si>
 </sst>
 </file>
@@ -472,10 +481,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="D2" t="n">
+        <v>15.0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -486,7 +495,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>30</v>

</xml_diff>

<commit_message>
Historia de Usuario 002 - arreglado creacion de nuevas hojas de excel
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Java Books" r:id="rId1" sheetId="1"/>
+    <sheet name="Java Books 2" r:id="rId5" sheetId="2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>No</t>
   </si>
@@ -129,6 +130,84 @@
   </si>
   <si>
     <t>Petrosky</t>
+  </si>
+  <si>
+    <t>Zzz</t>
+  </si>
+  <si>
+    <t>timmy</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>fff</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>uu</t>
+  </si>
+  <si>
+    <t>jj</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>pp</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>gg</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>vv</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>oo</t>
   </si>
 </sst>
 </file>
@@ -725,6 +804,189 @@
         <v>41.0</v>
       </c>
     </row>
+    <row r="20"/>
+    <row r="21">
+      <c r="B21" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>